<commit_message>
Add Readme and update excel
</commit_message>
<xml_diff>
--- a/docs/ScientificApplication/StealthCup_Timeline.xlsx
+++ b/docs/ScientificApplication/StealthCup_Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuel/Documents/projects/_dis-dev/StealthCup2025/docs/ScientificApplication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1D7AB9-CF79-1141-A1C6-F1BE590F4937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B622A27-5983-0044-933E-3C522D1C5D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20320" yWindow="3240" windowWidth="31260" windowHeight="24460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1147,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378BE20E-18C1-3F48-ABA4-55FA8CEC36DC}">
-  <dimension ref="A1:AA41"/>
+  <dimension ref="A1:AG41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1183,7 +1183,7 @@
     <col min="27" max="27" width="7.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="39"/>
       <c r="B1" s="40"/>
       <c r="C1" s="47" t="s">
@@ -1220,7 +1220,7 @@
       <c r="Z1" s="44"/>
       <c r="AA1" s="45"/>
     </row>
-    <row r="2" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="41"/>
       <c r="B2" s="42"/>
       <c r="C2" s="27" t="s">
@@ -1299,7 +1299,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="33">
         <v>1</v>
       </c>
@@ -1365,8 +1365,14 @@
         <f>X3+1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC3" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="35">
         <v>2</v>
       </c>
@@ -1436,8 +1442,11 @@
         <f t="shared" ref="AA4:AA14" si="5">X4+1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="35">
         <v>3</v>
       </c>
@@ -1511,8 +1520,11 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="35">
         <v>4</v>
       </c>
@@ -1580,8 +1592,11 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" s="35">
         <v>5</v>
       </c>
@@ -1635,8 +1650,11 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" s="35">
         <v>6</v>
       </c>
@@ -1700,8 +1718,11 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9" s="35">
         <v>7</v>
       </c>
@@ -1777,8 +1798,11 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" s="35">
         <v>8</v>
       </c>
@@ -1848,8 +1872,11 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" s="35">
         <v>9</v>
       </c>
@@ -1917,8 +1944,11 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" s="35">
         <v>10</v>
       </c>
@@ -1976,8 +2006,11 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" s="35">
         <v>11</v>
       </c>
@@ -2032,7 +2065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37">
         <v>12</v>
       </c>
@@ -2095,7 +2128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="V15" s="24">
         <f t="shared" ref="V15:Z15" si="6">SUM(V3:V14)</f>
         <v>16</v>
@@ -2195,15 +2228,16 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12B2AA47-AE15-214C-9B2C-8E4ADE4AC19E}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="A47" sqref="A47:A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2799,61 +2833,6 @@
       </c>
       <c r="D43" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>